<commit_message>
update fvfm and gene expression Rmd
</commit_message>
<xml_diff>
--- a/gene_expression/MS_bioinformatics/Bioinformatics/countreads.xlsx
+++ b/gene_expression/MS_bioinformatics/Bioinformatics/countreads.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.studivan/Downloads/allyson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_temperaturevariability2023/gene_expression/MS_bioinformatics/Bioinformatics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01ED9D7-3934-5140-85D1-FF5833A65028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="countreads" sheetId="8" r:id="rId1"/>
@@ -5264,86 +5264,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{646F0C16-19FD-624E-A296-17D029DF5848}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="O4:X5" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-    <i i="6">
-      <x v="6"/>
-    </i>
-    <i i="7">
-      <x v="7"/>
-    </i>
-    <i i="8">
-      <x v="8"/>
-    </i>
-    <i i="9">
-      <x v="9"/>
-    </i>
-  </colItems>
-  <dataFields count="10">
-    <dataField name="Average of Trimmed Reads Acer" fld="6" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Count of Trimmed Reads Acer2" fld="6" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="StdDev of Trimmed Reads Acer3" fld="6" subtotal="stdDev" baseField="0" baseItem="0"/>
-    <dataField name="Min of Trimmed Reads Acer4" fld="6" subtotal="min" baseField="0" baseItem="0"/>
-    <dataField name="Max of Trimmed Reads Acer5" fld="6" subtotal="max" baseField="0" baseItem="0"/>
-    <dataField name="Average of Trimmed Reads Pcli" fld="7" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Count of Trimmed Reads Pcli2" fld="7" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="StdDev of Trimmed Reads Pcli3" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
-    <dataField name="Min of Trimmed Reads Pcli4" fld="7" subtotal="min" baseField="0" baseItem="0"/>
-    <dataField name="Max of Trimmed Reads Pcli5" fld="7" subtotal="max" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31AD1DBE-A59C-1B4A-8D70-9C67B8C4610C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:BG2" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="13">
@@ -5550,6 +5470,86 @@
     <dataField name="StdDev of Alignment rate Pcli3" fld="12" subtotal="stdDev" baseField="0" baseItem="0"/>
     <dataField name="Min of Alignment rate Pcli4" fld="12" subtotal="min" baseField="0" baseItem="0"/>
     <dataField name="Max of Alignment rate Pcli5" fld="12" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{646F0C16-19FD-624E-A296-17D029DF5848}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="O4:X5" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+    <i i="7">
+      <x v="7"/>
+    </i>
+    <i i="8">
+      <x v="8"/>
+    </i>
+    <i i="9">
+      <x v="9"/>
+    </i>
+  </colItems>
+  <dataFields count="10">
+    <dataField name="Average of Trimmed Reads Acer" fld="6" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Count of Trimmed Reads Acer2" fld="6" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="StdDev of Trimmed Reads Acer3" fld="6" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="Min of Trimmed Reads Acer4" fld="6" subtotal="min" baseField="0" baseItem="0"/>
+    <dataField name="Max of Trimmed Reads Acer5" fld="6" subtotal="max" baseField="0" baseItem="0"/>
+    <dataField name="Average of Trimmed Reads Pcli" fld="7" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Count of Trimmed Reads Pcli2" fld="7" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="StdDev of Trimmed Reads Pcli3" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="Min of Trimmed Reads Pcli4" fld="7" subtotal="min" baseField="0" baseItem="0"/>
+    <dataField name="Max of Trimmed Reads Pcli5" fld="7" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -6002,8 +6002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ECAA35-E0BE-7A40-9657-06C681B0E3F4}">
   <dimension ref="A1:BG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10386,7 +10386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B025AEF7-F8A9-9C48-8415-0B12E655EDA8}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>

</xml_diff>